<commit_message>
update for new event
</commit_message>
<xml_diff>
--- a/Documents/journaux.xlsx
+++ b/Documents/journaux.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD9B1F2-0E12-4E84-BD26-4BDC47436FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0757F1CA-45CB-4F8C-9895-402C647A9DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="13920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de Board" sheetId="2" r:id="rId1"/>
     <sheet name="Feuil1" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Feuil1!$A:$D</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -90,13 +93,28 @@
   </si>
   <si>
     <t xml:space="preserve">visite 2em expert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">faire une modification sur la base de données un rendez-vous avec le chef de projet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint review 2 : clôture le sprint  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint review 3 : clôture le sprint  </t>
+  </si>
+  <si>
+    <t>3h01</t>
+  </si>
+  <si>
+    <t>2h00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +129,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -127,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -176,45 +213,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,12 +553,12 @@
       <selection activeCell="B26" sqref="B26:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="104.7265625" customWidth="1"/>
+    <col min="2" max="2" width="104.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>44683</v>
       </c>
@@ -522,7 +574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>44683</v>
       </c>
@@ -530,10 +582,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
         <v>44605</v>
       </c>
@@ -541,7 +593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
         <v>44624</v>
       </c>
@@ -549,7 +601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>44638</v>
       </c>
@@ -557,7 +609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>44641</v>
       </c>
@@ -573,155 +625,188 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="12.3828125" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
-    <col min="3" max="3" width="44.1796875" customWidth="1"/>
-    <col min="4" max="5" width="18.1796875" customWidth="1"/>
+    <col min="3" max="3" width="36.3046875" customWidth="1"/>
+    <col min="4" max="4" width="10.15234375" customWidth="1"/>
+    <col min="5" max="5" width="18.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="7">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="6">
         <v>44683</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7">
+    <row r="4" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="6">
         <v>44683</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7">
+    <row r="5" spans="1:4" ht="35.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="6">
         <v>44683</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" ht="45.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7">
+      <c r="C5" s="10"/>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="6">
         <v>44684</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7">
+      <c r="C6" s="10"/>
+      <c r="D6" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="6">
         <v>44684</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="8">
+      <c r="C7" s="10"/>
+      <c r="D7" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="56.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="11">
         <v>44686</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" ht="50.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="8">
+      <c r="C8" s="10"/>
+      <c r="D8" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="50.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="11">
         <v>44690</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="53.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7">
+    <row r="10" spans="1:4" ht="53.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="6">
         <v>44693</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7">
+    <row r="11" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="6">
         <v>44694</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="15">
+      <c r="C11" s="10"/>
+      <c r="D11" s="13">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
+    <row r="12" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="6">
+        <v>44705</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="14">
+        <v>44697</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="6">
+        <v>44712</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="13">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -730,7 +815,8 @@
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update my journal de board
</commit_message>
<xml_diff>
--- a/Documents/journaux.xlsx
+++ b/Documents/journaux.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0757F1CA-45CB-4F8C-9895-402C647A9DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4D9811-FA39-4A36-A20E-1691D4466608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="13920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de Board" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -77,9 +77,6 @@
     <t>1h00</t>
   </si>
   <si>
-    <t xml:space="preserve">un petit erreur au niveau gestion de temps  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sprint review 1 : clôture le sprint  </t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t xml:space="preserve">visite 2em expert </t>
   </si>
   <si>
-    <t xml:space="preserve">faire une modification sur la base de données un rendez-vous avec le chef de projet </t>
-  </si>
-  <si>
     <t xml:space="preserve">Sprint review 2 : clôture le sprint  </t>
   </si>
   <si>
@@ -108,6 +102,17 @@
   </si>
   <si>
     <t>2h00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un erreur au niveau gestion de temps  </t>
+  </si>
+  <si>
+    <t>Reunion avec l'expert + signature du cahier des charges de la part du 
+candidat durant la réunion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faire une modification sur la base de 
+données un rendez-vous avec le chef de projet </t>
   </si>
 </sst>
 </file>
@@ -228,17 +233,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -262,11 +261,22 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,12 +563,12 @@
       <selection activeCell="B26" sqref="B26:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.4609375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="104.69140625" customWidth="1"/>
+    <col min="2" max="2" width="104.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44683</v>
       </c>
@@ -574,7 +584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44683</v>
       </c>
@@ -582,10 +592,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44605</v>
       </c>
@@ -593,7 +603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44624</v>
       </c>
@@ -601,7 +611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>44638</v>
       </c>
@@ -609,7 +619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>44641</v>
       </c>
@@ -627,184 +637,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.3828125" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
-    <col min="3" max="3" width="36.3046875" customWidth="1"/>
-    <col min="4" max="4" width="10.15234375" customWidth="1"/>
-    <col min="5" max="5" width="18.15234375" customWidth="1"/>
+    <col min="3" max="3" width="36.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="6">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4">
         <v>44683</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4">
+        <v>44683</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6">
+    <row r="5" spans="1:4" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4">
         <v>44683</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4">
+        <v>44684</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4">
+        <v>44684</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9">
+        <v>44686</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="50.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9">
+        <v>44690</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="53.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="4">
+        <v>44693</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="4">
+        <v>44694</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="35.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="6">
-        <v>44683</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="6">
-        <v>44684</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="6">
-        <v>44684</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="56.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="11">
-        <v>44686</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="50.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="11">
-        <v>44690</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="53.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="6">
-        <v>44693</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="6">
-        <v>44694</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4">
+        <v>44705</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="13">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="6">
-        <v>44705</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="14">
+      <c r="C12" s="8"/>
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:4" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="12">
         <v>44697</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4">
+        <v>44712</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="16">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.9" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="6">
-        <v>44712</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="13">
+      <c r="C14" s="8"/>
+      <c r="D14" s="11">
         <v>60</v>
       </c>
     </row>

</xml_diff>